<commit_message>
tuned the fourier order. The best result so far is still moderate
</commit_message>
<xml_diff>
--- a/Robot RL2c/Tuning History.xlsx
+++ b/Robot RL2c/Tuning History.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -81,9 +81,6 @@
     <t>converge?</t>
   </si>
   <si>
-    <t>conv steps</t>
-  </si>
-  <si>
     <t>performance</t>
   </si>
   <si>
@@ -142,15 +139,47 @@
   </si>
   <si>
     <t>par.cost</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t>deviating</t>
+  </si>
+  <si>
+    <t>14:42 PM</t>
+  </si>
+  <si>
+    <t>stopped at around 250th trial due to instability induced by sudden leap in the alpha. This can be used for further tuning</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>so so</t>
+  </si>
+  <si>
+    <t>alfa filter coeff</t>
+  </si>
+  <si>
+    <t>1/300?? (fail!)</t>
+  </si>
+  <si>
+    <t>x10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
-    <numFmt numFmtId="167" formatCode="0.000E+00"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -378,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -415,11 +444,15 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,7 +837,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -1089,13 +1122,15 @@
   <dimension ref="B1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1104,9 +1139,15 @@
       <c r="C1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="D1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>10</v>
+      </c>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
@@ -1120,11 +1161,17 @@
         <v>1</v>
       </c>
       <c r="C2" s="9">
-        <v>42130</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+        <v>42131</v>
+      </c>
+      <c r="D2" s="9">
+        <v>42131</v>
+      </c>
+      <c r="E2" s="24">
+        <v>42131</v>
+      </c>
+      <c r="F2" s="24">
+        <v>42131</v>
+      </c>
       <c r="G2" s="24"/>
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
@@ -1138,11 +1185,17 @@
         <v>2</v>
       </c>
       <c r="C3" s="26">
-        <v>0.46527777777777773</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+        <v>0.49583333333333335</v>
+      </c>
+      <c r="D3" s="36">
+        <v>0.4993055555555555</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="36">
+        <v>0.69652777777777775</v>
+      </c>
       <c r="G3" s="11"/>
       <c r="H3" s="25"/>
       <c r="I3" s="11"/>
@@ -1174,26 +1227,50 @@
       <c r="C5" s="27">
         <v>500</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="29"/>
+      <c r="D5" s="27">
+        <v>500</v>
+      </c>
+      <c r="E5" s="27">
+        <v>500</v>
+      </c>
+      <c r="F5" s="27">
+        <v>500</v>
+      </c>
+      <c r="G5" s="27">
+        <v>500</v>
+      </c>
+      <c r="H5" s="27">
+        <v>500</v>
+      </c>
+      <c r="I5" s="27">
+        <v>500</v>
+      </c>
+      <c r="J5" s="27">
+        <v>500</v>
+      </c>
+      <c r="K5" s="27">
+        <v>500</v>
+      </c>
+      <c r="L5" s="27">
+        <v>500</v>
+      </c>
+      <c r="M5" s="27">
+        <v>500</v>
+      </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="27">
-        <v>4</v>
-      </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+        <v>6</v>
+      </c>
+      <c r="D6" s="27">
+        <v>6</v>
+      </c>
+      <c r="E6" s="27">
+        <v>6</v>
+      </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
@@ -1205,13 +1282,17 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="27">
-        <v>4</v>
-      </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+        <v>6</v>
+      </c>
+      <c r="D7" s="27">
+        <v>6</v>
+      </c>
+      <c r="E7" s="27">
+        <v>6</v>
+      </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
@@ -1223,13 +1304,17 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="28">
-        <v>0.01</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+        <v>27</v>
+      </c>
+      <c r="C8" s="33">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="D8" s="33">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="E8" s="33">
+        <v>5.0000000000000002E-5</v>
+      </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
@@ -1241,13 +1326,17 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="28">
-        <v>1E-4</v>
-      </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
+        <v>28</v>
+      </c>
+      <c r="C9" s="33">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="D9" s="33">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="E9" s="33">
+        <v>5.0000000000000002E-5</v>
+      </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
@@ -1259,13 +1348,17 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
+        <v>38</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
@@ -1277,13 +1370,17 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
+        <v>38</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
@@ -1295,13 +1392,17 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="28">
+        <v>31</v>
+      </c>
+      <c r="C12" s="34">
         <v>1</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
+      <c r="D12" s="34">
+        <v>1.3</v>
+      </c>
+      <c r="E12" s="34">
+        <v>2</v>
+      </c>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
@@ -1313,13 +1414,17 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="28">
-        <v>1</v>
-      </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
+        <v>32</v>
+      </c>
+      <c r="C13" s="34">
+        <v>3</v>
+      </c>
+      <c r="D13" s="34">
+        <v>3</v>
+      </c>
+      <c r="E13" s="34">
+        <v>2</v>
+      </c>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
@@ -1331,13 +1436,17 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="32">
-        <v>100000000</v>
-      </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
+        <v>33</v>
+      </c>
+      <c r="C14" s="35">
+        <v>1000</v>
+      </c>
+      <c r="D14" s="35">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="35">
+        <v>1000</v>
+      </c>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
@@ -1349,13 +1458,17 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
+        <v>34</v>
+      </c>
+      <c r="C15" s="27">
+        <v>100</v>
+      </c>
+      <c r="D15" s="27">
+        <v>100</v>
+      </c>
+      <c r="E15" s="27">
+        <v>100</v>
+      </c>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
@@ -1367,13 +1480,17 @@
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="28">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
+        <v>35</v>
+      </c>
+      <c r="C16" s="32">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D16" s="32">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E16" s="32">
+        <v>8.9999999999999993E-3</v>
+      </c>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
@@ -1385,13 +1502,17 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="28">
+        <v>36</v>
+      </c>
+      <c r="C17" s="32">
         <v>1E-4</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
+      <c r="D17" s="32">
+        <v>1E-4</v>
+      </c>
+      <c r="E17" s="32">
+        <v>1E-4</v>
+      </c>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
@@ -1403,13 +1524,17 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="28">
+        <v>37</v>
+      </c>
+      <c r="C18" s="32">
         <v>1</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
+      <c r="D18" s="32">
+        <v>1</v>
+      </c>
+      <c r="E18" s="32">
+        <v>1</v>
+      </c>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
@@ -1421,13 +1546,17 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="28">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
+        <v>39</v>
+      </c>
+      <c r="C19" s="32">
+        <v>0.97</v>
+      </c>
+      <c r="D19" s="32">
+        <v>0.97</v>
+      </c>
+      <c r="E19" s="32">
+        <v>0.97</v>
+      </c>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
@@ -1439,14 +1568,20 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
+      <c r="D20" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>15</v>
+      </c>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
@@ -1489,9 +1624,15 @@
       <c r="B23" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="C23" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
@@ -1503,11 +1644,17 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
@@ -1519,11 +1666,17 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -1535,11 +1688,13 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
+      <c r="E26" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
@@ -1551,12 +1706,16 @@
     </row>
     <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="7" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
+      <c r="E27" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>50</v>
+      </c>
       <c r="G27" s="18"/>
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>

</xml_diff>

<commit_message>
made an independent period for the fourier basis function. More tuning is needed
</commit_message>
<xml_diff>
--- a/Robot RL2c/Tuning History.xlsx
+++ b/Robot RL2c/Tuning History.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -168,7 +168,28 @@
     <t>1/300?? (fail!)</t>
   </si>
   <si>
-    <t>x10</t>
+    <t>after overshooting, it keeps on deviating from the reference</t>
+  </si>
+  <si>
+    <t>actor approx</t>
+  </si>
+  <si>
+    <t>critic approx</t>
+  </si>
+  <si>
+    <t>cos</t>
+  </si>
+  <si>
+    <t>cos &amp; sine</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>the additive input is coarse, damaging the td</t>
+  </si>
+  <si>
+    <t>the input is still coarse due to the large variance across zdot space</t>
   </si>
 </sst>
 </file>
@@ -177,9 +198,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -407,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -441,16 +462,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -1119,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M27"/>
+  <dimension ref="B1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1130,8 +1150,8 @@
     <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.3">
@@ -1170,10 +1190,14 @@
         <v>42131</v>
       </c>
       <c r="F2" s="24">
-        <v>42131</v>
-      </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+        <v>42135</v>
+      </c>
+      <c r="G2" s="24">
+        <v>42135</v>
+      </c>
+      <c r="H2" s="24">
+        <v>42135</v>
+      </c>
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
       <c r="K2" s="12"/>
@@ -1184,20 +1208,24 @@
       <c r="B3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="25">
         <v>0.49583333333333335</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="35">
         <v>0.4993055555555555</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="36">
-        <v>0.69652777777777775</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="25"/>
+      <c r="F3" s="35">
+        <v>0.48402777777777778</v>
+      </c>
+      <c r="G3" s="35">
+        <v>0.55972222222222223</v>
+      </c>
+      <c r="H3" s="35">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
@@ -1224,37 +1252,37 @@
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="26">
         <v>500</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="26">
         <v>500</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="26">
         <v>500</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="26">
         <v>500</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="26">
         <v>500</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="26">
         <v>500</v>
       </c>
-      <c r="I5" s="27">
+      <c r="I5" s="26">
         <v>500</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J5" s="26">
         <v>500</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="26">
         <v>500</v>
       </c>
-      <c r="L5" s="27">
+      <c r="L5" s="26">
         <v>500</v>
       </c>
-      <c r="M5" s="27">
+      <c r="M5" s="26">
         <v>500</v>
       </c>
     </row>
@@ -1262,377 +1290,473 @@
       <c r="B6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <v>6</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <v>6</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <v>6</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="29"/>
+      <c r="F6" s="26">
+        <v>6</v>
+      </c>
+      <c r="G6" s="26">
+        <v>6</v>
+      </c>
+      <c r="H6" s="27">
+        <v>4</v>
+      </c>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="28"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="26">
         <v>6</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="26">
         <v>6</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <v>6</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="29"/>
+      <c r="F7" s="26">
+        <v>6</v>
+      </c>
+      <c r="G7" s="26">
+        <v>6</v>
+      </c>
+      <c r="H7" s="27">
+        <v>4</v>
+      </c>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="28"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="32">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="32">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="32">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="29"/>
+      <c r="F8" s="27">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G8" s="27">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="H8" s="27">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="28"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="32">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="32">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="32">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="29"/>
+      <c r="F9" s="27">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="G9" s="27">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="H9" s="27">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="28"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="29"/>
+      <c r="F10" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="28"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="29"/>
+      <c r="F11" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="28"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="34">
+      <c r="C12" s="33">
         <v>1</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="33">
         <v>1.3</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="33">
         <v>2</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="29"/>
+      <c r="F12" s="33">
+        <v>2</v>
+      </c>
+      <c r="G12" s="33">
+        <v>2</v>
+      </c>
+      <c r="H12" s="33">
+        <v>2</v>
+      </c>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="28"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="33">
         <v>3</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="33">
         <v>3</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="33">
         <v>2</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="29"/>
+      <c r="F13" s="33">
+        <v>3</v>
+      </c>
+      <c r="G13" s="33">
+        <v>2</v>
+      </c>
+      <c r="H13" s="33">
+        <v>2</v>
+      </c>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="28"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="34">
         <v>1000</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="34">
         <v>1000</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="34">
         <v>1000</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="29"/>
+      <c r="F14" s="34">
+        <v>1000</v>
+      </c>
+      <c r="G14" s="34">
+        <v>1000</v>
+      </c>
+      <c r="H14" s="34">
+        <v>1000</v>
+      </c>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="28"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="26">
         <v>100</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="26">
         <v>100</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="26">
         <v>100</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="29"/>
+      <c r="F15" s="26">
+        <v>100</v>
+      </c>
+      <c r="G15" s="26">
+        <v>100</v>
+      </c>
+      <c r="H15" s="26">
+        <v>100</v>
+      </c>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="28"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="31">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="31">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="31">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="29"/>
+      <c r="F16" s="31">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G16" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="H16" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="28"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="31">
         <v>1E-4</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="31">
         <v>1E-4</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="31">
         <v>1E-4</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="29"/>
+      <c r="F17" s="31">
+        <v>1E-4</v>
+      </c>
+      <c r="G17" s="31">
+        <v>1E-4</v>
+      </c>
+      <c r="H17" s="31">
+        <v>1E-4</v>
+      </c>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="28"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="31">
         <v>1</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="31">
         <v>1</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="31">
         <v>1</v>
       </c>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="29"/>
+      <c r="F18" s="31">
+        <v>1</v>
+      </c>
+      <c r="G18" s="31">
+        <v>1</v>
+      </c>
+      <c r="H18" s="31">
+        <v>1</v>
+      </c>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="28"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="31">
         <v>0.97</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="31">
         <v>0.97</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="31">
         <v>0.97</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="29"/>
+      <c r="F19" s="31">
+        <v>0.97</v>
+      </c>
+      <c r="G19" s="31">
+        <v>0.97</v>
+      </c>
+      <c r="H19" s="31">
+        <v>0.99</v>
+      </c>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="28"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="29"/>
+      <c r="G20" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="28"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="14"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="31"/>
+      <c r="B21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="28"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="30"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="17"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
@@ -1644,20 +1768,26 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+        <v>46</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -1666,20 +1796,26 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
+        <v>47</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -1688,41 +1824,83 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="E26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="17"/>
     </row>
-    <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="7" t="s">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="17"/>
+    </row>
+    <row r="28" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18" t="s">
+      <c r="C28" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="19"/>
+      <c r="F28" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
the fourier based RL is finally showing a good, though still not as good as the z only controller
</commit_message>
<xml_diff>
--- a/Robot RL2c/Tuning History.xlsx
+++ b/Robot RL2c/Tuning History.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -190,6 +190,51 @@
   </si>
   <si>
     <t>the input is still coarse due to the large variance across zdot space</t>
+  </si>
+  <si>
+    <t>[2 6]</t>
+  </si>
+  <si>
+    <t>yes, but eventually diverged after 300 iteration</t>
+  </si>
+  <si>
+    <t>the input is no longer coarse since the penalty on zdot is reduced dramatically</t>
+  </si>
+  <si>
+    <t>rather good</t>
+  </si>
+  <si>
+    <t>critic initialization</t>
+  </si>
+  <si>
+    <t>optimistic</t>
+  </si>
+  <si>
+    <t>stopped at the middle of the experimet since the trajectory go outside the defined region and the input as well as temporal difference become coarse (oscillating)</t>
+  </si>
+  <si>
+    <t>stopped at the middle of the experimet since the trajectory deviates</t>
+  </si>
+  <si>
+    <t>[2 10]</t>
+  </si>
+  <si>
+    <t>the first duration (0-2s) trajectory is improved dramatically while the ending is not. The result is an unbalance diagonal-like trajectory. Conclusion: increasing zdot period and decreasing actor fourier basis order is making the learning worse</t>
+  </si>
+  <si>
+    <t>Trial 7</t>
+  </si>
+  <si>
+    <t>Trial 8</t>
+  </si>
+  <si>
+    <t>Trial 9</t>
+  </si>
+  <si>
+    <t>Trial 10</t>
+  </si>
+  <si>
+    <t>Trial 11</t>
   </si>
 </sst>
 </file>
@@ -233,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -299,13 +344,24 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -316,30 +372,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -363,31 +395,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -428,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,29 +458,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1139,104 +1144,139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B1" s="21"/>
-      <c r="C1" s="22" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="D1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="E1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-    </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="F1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="9">
+        <v>42131</v>
       </c>
       <c r="C2" s="9">
         <v>42131</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="21">
         <v>42131</v>
       </c>
-      <c r="E2" s="24">
-        <v>42131</v>
-      </c>
-      <c r="F2" s="24">
+      <c r="E2" s="21">
         <v>42135</v>
       </c>
-      <c r="G2" s="24">
+      <c r="F2" s="21">
         <v>42135</v>
       </c>
-      <c r="H2" s="24">
+      <c r="G2" s="21">
         <v>42135</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="13"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+      <c r="H2" s="21">
+        <v>42136</v>
+      </c>
+      <c r="I2" s="21">
+        <v>42136</v>
+      </c>
+      <c r="J2" s="31">
+        <v>42136</v>
+      </c>
+      <c r="K2" s="31">
+        <v>42136</v>
+      </c>
+      <c r="L2" s="32">
+        <v>42136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="25">
+      <c r="B3" s="22">
         <v>0.49583333333333335</v>
       </c>
-      <c r="D3" s="35">
+      <c r="C3" s="30">
         <v>0.4993055555555555</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="35">
+      <c r="E3" s="30">
         <v>0.48402777777777778</v>
       </c>
-      <c r="G3" s="35">
+      <c r="F3" s="30">
         <v>0.55972222222222223</v>
       </c>
-      <c r="H3" s="35">
+      <c r="G3" s="30">
         <v>0.70833333333333337</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="15"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="16" t="s">
+      <c r="H3" s="30">
+        <v>0.46249999999999997</v>
+      </c>
+      <c r="I3" s="30">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="J3" s="30">
+        <v>0.61249999999999993</v>
+      </c>
+      <c r="K3" s="30">
+        <v>0.63611111111111118</v>
+      </c>
+      <c r="L3" s="15"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -1245,515 +1285,685 @@
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="13"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="L4" s="13"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="26">
+      <c r="B5" s="23">
         <v>500</v>
       </c>
-      <c r="D5" s="26">
+      <c r="C5" s="23">
         <v>500</v>
       </c>
-      <c r="E5" s="26">
+      <c r="D5" s="23">
         <v>500</v>
       </c>
-      <c r="F5" s="26">
+      <c r="E5" s="23">
         <v>500</v>
       </c>
-      <c r="G5" s="26">
+      <c r="F5" s="23">
         <v>500</v>
       </c>
-      <c r="H5" s="26">
+      <c r="G5" s="23">
         <v>500</v>
       </c>
-      <c r="I5" s="26">
+      <c r="H5" s="23">
         <v>500</v>
       </c>
-      <c r="J5" s="26">
+      <c r="I5" s="23">
         <v>500</v>
       </c>
-      <c r="K5" s="26">
+      <c r="J5" s="23">
         <v>500</v>
       </c>
-      <c r="L5" s="26">
+      <c r="K5" s="23">
         <v>500</v>
       </c>
-      <c r="M5" s="26">
+      <c r="L5" s="23">
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="26">
+      <c r="B6" s="23">
         <v>6</v>
       </c>
-      <c r="D6" s="26">
+      <c r="C6" s="23">
         <v>6</v>
       </c>
-      <c r="E6" s="26">
+      <c r="D6" s="23">
         <v>6</v>
       </c>
-      <c r="F6" s="26">
+      <c r="E6" s="23">
         <v>6</v>
       </c>
-      <c r="G6" s="26">
+      <c r="F6" s="23">
         <v>6</v>
       </c>
-      <c r="H6" s="27">
+      <c r="G6" s="23">
         <v>4</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
+      <c r="H6" s="23">
+        <v>4</v>
+      </c>
+      <c r="I6" s="23">
+        <v>4</v>
+      </c>
+      <c r="J6" s="23">
+        <v>6</v>
+      </c>
+      <c r="K6" s="23">
+        <v>6</v>
+      </c>
+      <c r="L6" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="26">
+      <c r="B7" s="23">
         <v>6</v>
       </c>
-      <c r="D7" s="26">
+      <c r="C7" s="23">
         <v>6</v>
       </c>
-      <c r="E7" s="26">
+      <c r="D7" s="23">
         <v>6</v>
       </c>
-      <c r="F7" s="26">
+      <c r="E7" s="23">
         <v>6</v>
       </c>
-      <c r="G7" s="26">
+      <c r="F7" s="23">
         <v>6</v>
       </c>
-      <c r="H7" s="27">
+      <c r="G7" s="23">
         <v>4</v>
       </c>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="28"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+      <c r="H7" s="23">
+        <v>4</v>
+      </c>
+      <c r="I7" s="23">
+        <v>4</v>
+      </c>
+      <c r="J7" s="23">
+        <v>6</v>
+      </c>
+      <c r="K7" s="23">
+        <v>4</v>
+      </c>
+      <c r="L7" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="32">
+      <c r="B8" s="27">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="D8" s="32">
+      <c r="C8" s="27">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="E8" s="32">
+      <c r="D8" s="27">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="F8" s="27">
+      <c r="E8" s="24">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G8" s="27">
+      <c r="F8" s="24">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="H8" s="27">
+      <c r="G8" s="24">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="28"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
+      <c r="H8" s="24">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I8" s="24">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J8" s="24">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K8" s="24">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L8" s="24">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="32">
+      <c r="B9" s="27">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="D9" s="32">
+      <c r="C9" s="27">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="E9" s="32">
+      <c r="D9" s="27">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="F9" s="27">
+      <c r="E9" s="24">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="G9" s="27">
+      <c r="F9" s="24">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="H9" s="27">
+      <c r="G9" s="24">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="28"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
+      <c r="H9" s="24">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="I9" s="24">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="J9" s="24">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="K9" s="24">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="L9" s="24">
+        <v>5.0000000000000004E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="B10" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="C10" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="D10" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="E10" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="F10" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="G10" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="28"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+      <c r="H10" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="B11" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="C11" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="D11" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="E11" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="F11" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="G11" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="28"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
+      <c r="H11" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="33">
+      <c r="B12" s="28">
         <v>1</v>
       </c>
-      <c r="D12" s="33">
+      <c r="C12" s="28">
         <v>1.3</v>
       </c>
-      <c r="E12" s="33">
+      <c r="D12" s="28">
         <v>2</v>
       </c>
-      <c r="F12" s="33">
+      <c r="E12" s="28">
         <v>2</v>
       </c>
-      <c r="G12" s="33">
+      <c r="F12" s="28">
         <v>2</v>
       </c>
-      <c r="H12" s="33">
+      <c r="G12" s="28">
         <v>2</v>
       </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="28"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
+      <c r="H12" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="33">
+      <c r="B13" s="28">
         <v>3</v>
       </c>
-      <c r="D13" s="33">
+      <c r="C13" s="28">
         <v>3</v>
       </c>
-      <c r="E13" s="33">
+      <c r="D13" s="28">
         <v>2</v>
       </c>
-      <c r="F13" s="33">
+      <c r="E13" s="28">
         <v>3</v>
       </c>
-      <c r="G13" s="33">
+      <c r="F13" s="28">
         <v>2</v>
       </c>
-      <c r="H13" s="33">
+      <c r="G13" s="28">
         <v>2</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="28"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
+      <c r="H13" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="34">
+      <c r="B14" s="29">
         <v>1000</v>
       </c>
-      <c r="D14" s="34">
+      <c r="C14" s="29">
         <v>1000</v>
       </c>
-      <c r="E14" s="34">
+      <c r="D14" s="29">
         <v>1000</v>
       </c>
-      <c r="F14" s="34">
+      <c r="E14" s="29">
         <v>1000</v>
       </c>
-      <c r="G14" s="34">
+      <c r="F14" s="29">
         <v>1000</v>
       </c>
-      <c r="H14" s="34">
+      <c r="G14" s="29">
         <v>1000</v>
       </c>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="28"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="6" t="s">
+      <c r="H14" s="29">
+        <v>1000</v>
+      </c>
+      <c r="I14" s="29">
+        <v>1000</v>
+      </c>
+      <c r="J14" s="29">
+        <v>1000</v>
+      </c>
+      <c r="K14" s="29">
+        <v>1000</v>
+      </c>
+      <c r="L14" s="29">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="26">
+      <c r="B15" s="23">
         <v>100</v>
       </c>
-      <c r="D15" s="26">
+      <c r="C15" s="23">
         <v>100</v>
       </c>
-      <c r="E15" s="26">
+      <c r="D15" s="23">
         <v>100</v>
       </c>
-      <c r="F15" s="26">
+      <c r="E15" s="23">
         <v>100</v>
       </c>
-      <c r="G15" s="26">
+      <c r="F15" s="23">
         <v>100</v>
       </c>
-      <c r="H15" s="26">
+      <c r="G15" s="23">
         <v>100</v>
       </c>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="28"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
+      <c r="H15" s="23">
+        <v>1</v>
+      </c>
+      <c r="I15" s="23">
+        <v>1</v>
+      </c>
+      <c r="J15" s="23">
+        <v>1</v>
+      </c>
+      <c r="K15" s="23">
+        <v>1</v>
+      </c>
+      <c r="L15" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="31">
+      <c r="B16" s="26">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="D16" s="31">
+      <c r="C16" s="26">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E16" s="31">
+      <c r="D16" s="26">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F16" s="31">
+      <c r="E16" s="26">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G16" s="31">
+      <c r="F16" s="26">
         <v>0.01</v>
       </c>
-      <c r="H16" s="27">
+      <c r="G16" s="24">
         <v>0.01</v>
       </c>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="28"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="6" t="s">
+      <c r="H16" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="I16" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="J16" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="K16" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="L16" s="24">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="31">
+      <c r="B17" s="26">
         <v>1E-4</v>
       </c>
-      <c r="D17" s="31">
+      <c r="C17" s="26">
         <v>1E-4</v>
       </c>
-      <c r="E17" s="31">
+      <c r="D17" s="26">
         <v>1E-4</v>
       </c>
-      <c r="F17" s="31">
+      <c r="E17" s="26">
         <v>1E-4</v>
       </c>
-      <c r="G17" s="31">
+      <c r="F17" s="26">
         <v>1E-4</v>
       </c>
-      <c r="H17" s="31">
+      <c r="G17" s="26">
         <v>1E-4</v>
       </c>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="28"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="6" t="s">
+      <c r="H17" s="26">
+        <v>1E-4</v>
+      </c>
+      <c r="I17" s="26">
+        <v>1E-4</v>
+      </c>
+      <c r="J17" s="26">
+        <v>1E-4</v>
+      </c>
+      <c r="K17" s="26">
+        <v>1E-4</v>
+      </c>
+      <c r="L17" s="26">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="31">
+      <c r="B18" s="26">
         <v>1</v>
       </c>
-      <c r="D18" s="31">
+      <c r="C18" s="26">
         <v>1</v>
       </c>
-      <c r="E18" s="31">
+      <c r="D18" s="26">
         <v>1</v>
       </c>
-      <c r="F18" s="31">
+      <c r="E18" s="26">
         <v>1</v>
       </c>
-      <c r="G18" s="31">
+      <c r="F18" s="26">
         <v>1</v>
       </c>
-      <c r="H18" s="31">
+      <c r="G18" s="26">
         <v>1</v>
       </c>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="28"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
+      <c r="H18" s="26">
+        <v>1</v>
+      </c>
+      <c r="I18" s="26">
+        <v>1</v>
+      </c>
+      <c r="J18" s="26">
+        <v>1</v>
+      </c>
+      <c r="K18" s="26">
+        <v>1</v>
+      </c>
+      <c r="L18" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="31">
+      <c r="B19" s="26">
         <v>0.97</v>
       </c>
-      <c r="D19" s="31">
+      <c r="C19" s="26">
         <v>0.97</v>
       </c>
-      <c r="E19" s="31">
+      <c r="D19" s="26">
         <v>0.97</v>
       </c>
-      <c r="F19" s="31">
+      <c r="E19" s="26">
         <v>0.97</v>
       </c>
-      <c r="G19" s="31">
+      <c r="F19" s="26">
         <v>0.97</v>
       </c>
-      <c r="H19" s="31">
+      <c r="G19" s="26">
         <v>0.99</v>
       </c>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="28"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="6" t="s">
+      <c r="H19" s="26">
+        <v>0.99</v>
+      </c>
+      <c r="I19" s="26">
+        <v>0.99</v>
+      </c>
+      <c r="J19" s="26">
+        <v>0.99</v>
+      </c>
+      <c r="K19" s="26">
+        <v>0.99</v>
+      </c>
+      <c r="L19" s="26">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="B20" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="C20" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="D20" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="E20" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="27" t="s">
+      <c r="F20" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="G20" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="28"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
+      <c r="H20" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27" t="s">
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="F21" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="G21" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="28"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
+      <c r="H21" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21" s="25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29" t="s">
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="F22" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="G22" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="30"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="5" t="s">
+      <c r="H22" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J22" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K22" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="L22" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -1764,51 +1974,63 @@
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="17"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>20</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D24" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="F24" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>41</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>46</v>
       </c>
       <c r="H24" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="17"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
+      <c r="J24" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L24" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="B25" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="C25" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="F25" s="10" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>55</v>
@@ -1816,15 +2038,25 @@
       <c r="H25" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="17"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
+      <c r="I25" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L25" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
         <v>23</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>15</v>
@@ -1844,63 +2076,126 @@
       <c r="H26" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="17"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="6" t="s">
+      <c r="I26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="B27" s="10"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
+      <c r="D27" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="E27" s="10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="17"/>
-    </row>
-    <row r="28" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="7" t="s">
+      <c r="J27" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L27" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="B29" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="C29" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="D29" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="E29" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="G28" s="18" t="s">
+      <c r="F29" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H28" s="18" t="s">
+      <c r="G29" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="19"/>
+      <c r="H29" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J29" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>